<commit_message>
0724 2:30PM REST api Excel
</commit_message>
<xml_diff>
--- a/src/main/java/web/REST api 명세서와 개발순서.xlsx
+++ b/src/main/java/web/REST api 명세서와 개발순서.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tj-bu-703-15\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E4E969-5923-4F09-995E-9906627E3982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D21325FF-75B9-4F9C-8AA3-F310424AE902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{79D24F31-FD52-4199-9C23-A523360A35DE}"/>
+    <workbookView xWindow="135" yWindow="90" windowWidth="22335" windowHeight="12930" xr2:uid="{79D24F31-FD52-4199-9C23-A523360A35DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="76">
   <si>
     <t>REST API 명세서</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -88,10 +88,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>글 전체 호출 처리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>글 상세 호출 처리</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -108,10 +104,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>글 전체 페이지 요청</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>글 상세 페이지 요청</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -293,6 +285,54 @@
   </si>
   <si>
     <t>윤성연</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>글 전체 호출 처리 및 페이지 요청</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boardgetall.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boardread.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boardedit.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(순번 3번과 중복) 글 전체 페이지 요청</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boardwrite.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>게시판전체출력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>게시판상세글</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>게시글수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>게시글작성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>페이지 기능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HTML 주소</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -397,22 +437,22 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -456,23 +496,34 @@
   </sortState>
   <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{71AF3709-512B-415A-9603-158D5089D5D9}" name="순번" dataDxfId="15"/>
-    <tableColumn id="19" xr3:uid="{6D6BEAD2-DA9F-464E-9E54-34D02D201488}" name="개발순서" dataDxfId="1"/>
-    <tableColumn id="17" xr3:uid="{8DB94640-D242-4CA1-B641-9EF58787951B}" name="완성여부" dataDxfId="2"/>
-    <tableColumn id="16" xr3:uid="{8CD32B70-1DAF-4DCA-A9BC-54743CC9DF6E}" name="백엔드" dataDxfId="3"/>
-    <tableColumn id="15" xr3:uid="{92EF7625-BEDC-4749-8539-16419660326F}" name="프론트엔드" dataDxfId="4"/>
-    <tableColumn id="20" xr3:uid="{DB691279-9B34-4B5C-9BF3-2C49D305395F}" name="명세서담당" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{BADCDF08-0FCA-44D9-970B-4E0D9850F9D9}" name="설명" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{F74AEC18-21BF-4EAD-A56D-68257D0D71D2}" name="HTTP method" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{79F026B3-A7F5-4EF6-B424-F8EF9E8734BF}" name="HTTP url" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{A57FB909-E924-4F78-A1CD-5A6FF0088AC9}" name="HTTP request contentType" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{518AB64C-D968-4741-9D44-FD84CDA875F1}" name="HTTP request data" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{E740BC06-8F9D-4CDD-8CBB-AA0CA1E0F308}" name="request 어노테이션" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{0D61888C-71A0-4B2E-8AF0-34E785CB0BBF}" name="HTTP response contentType" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{2578BB80-2EC2-4AD9-A49B-B4C14F33CAC7}" name="HTTP response data" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{B00D3CD9-F826-408F-9300-7A27991B9701}" name="Model and View" dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{B58F5F64-0EA3-4DCF-AE42-3BE1CC84CA65}" name="response 어노테이션" dataDxfId="5"/>
+    <tableColumn id="19" xr3:uid="{6D6BEAD2-DA9F-464E-9E54-34D02D201488}" name="개발순서" dataDxfId="14"/>
+    <tableColumn id="17" xr3:uid="{8DB94640-D242-4CA1-B641-9EF58787951B}" name="완성여부" dataDxfId="13"/>
+    <tableColumn id="16" xr3:uid="{8CD32B70-1DAF-4DCA-A9BC-54743CC9DF6E}" name="백엔드" dataDxfId="12"/>
+    <tableColumn id="15" xr3:uid="{92EF7625-BEDC-4749-8539-16419660326F}" name="프론트엔드" dataDxfId="11"/>
+    <tableColumn id="20" xr3:uid="{DB691279-9B34-4B5C-9BF3-2C49D305395F}" name="명세서담당" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{BADCDF08-0FCA-44D9-970B-4E0D9850F9D9}" name="설명" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{F74AEC18-21BF-4EAD-A56D-68257D0D71D2}" name="HTTP method" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{79F026B3-A7F5-4EF6-B424-F8EF9E8734BF}" name="HTTP url" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{A57FB909-E924-4F78-A1CD-5A6FF0088AC9}" name="HTTP request contentType" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{518AB64C-D968-4741-9D44-FD84CDA875F1}" name="HTTP request data" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{E740BC06-8F9D-4CDD-8CBB-AA0CA1E0F308}" name="request 어노테이션" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{0D61888C-71A0-4B2E-8AF0-34E785CB0BBF}" name="HTTP response contentType" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{2578BB80-2EC2-4AD9-A49B-B4C14F33CAC7}" name="HTTP response data" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{B00D3CD9-F826-408F-9300-7A27991B9701}" name="Model and View" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{B58F5F64-0EA3-4DCF-AE42-3BE1CC84CA65}" name="response 어노테이션" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{39162907-BBD6-4C32-81BE-7D935531BFFC}" name="표2" displayName="표2" ref="C22:D26" totalsRowShown="0">
+  <autoFilter ref="C22:D26" xr:uid="{39162907-BBD6-4C32-81BE-7D935531BFFC}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{50C11E6D-577B-42F8-81F8-6DE8A248D9DF}" name="페이지 기능"/>
+    <tableColumn id="2" xr3:uid="{658DEB4F-DF79-4519-B83B-591D91C5B96A}" name="HTML 주소"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -773,21 +824,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3369F36A-6395-48DF-8E97-C2FF2FC0F556}">
-  <dimension ref="B2:R20"/>
+  <dimension ref="B2:R26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.375" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="3" max="3" width="15.625" customWidth="1"/>
+    <col min="4" max="4" width="18.875" customWidth="1"/>
     <col min="5" max="5" width="12.375" customWidth="1"/>
     <col min="6" max="6" width="13.375" customWidth="1"/>
     <col min="7" max="7" width="13.125" customWidth="1"/>
-    <col min="8" max="8" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="56" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="31.125" bestFit="1" customWidth="1"/>
@@ -825,19 +876,19 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>2</v>
@@ -879,42 +930,42 @@
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="I4" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="P4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q4" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="R4" s="1"/>
     </row>
@@ -923,40 +974,40 @@
         <v>8</v>
       </c>
       <c r="C5" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="H5" s="1" t="s">
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="O5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P5" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
@@ -969,227 +1020,227 @@
         <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="H6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="K6" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="P6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q6" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="7" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C7" s="1">
         <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="H7" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
       <c r="N7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="P7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>40</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="Q7" s="1"/>
     </row>
     <row r="8" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C8" s="1">
         <v>5</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>63</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="N8" s="1" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q8" s="1"/>
+        <v>36</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="9" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="1">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C9" s="1">
         <v>6</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="G9" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L9" s="1"/>
+        <v>47</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="M9" s="1"/>
       <c r="N9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="O9" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="P9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q9" s="1" t="s">
-        <v>40</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="Q9" s="1"/>
     </row>
     <row r="10" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="1">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C10" s="1">
         <v>7</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>63</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>50</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q10" s="1"/>
+        <v>36</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="11" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="1">
@@ -1199,166 +1250,206 @@
         <v>8</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="H11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K11" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="P11" s="1" t="s">
+      <c r="Q11" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="Q11" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="12" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C12" s="1">
         <v>9</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>63</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="M12" s="1"/>
       <c r="N12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="O12" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="P12" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q12" s="1" t="s">
-        <v>40</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="Q12" s="1"/>
     </row>
     <row r="13" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C13" s="1">
         <v>10</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="G13" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K13" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="L13" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="M13" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="N13" s="1" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q13" s="1"/>
+        <v>36</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.3">
       <c r="D15" t="s">
+        <v>56</v>
+      </c>
+      <c r="H15" t="s">
         <v>58</v>
-      </c>
-      <c r="H15" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.3">
       <c r="D16" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D18" t="s">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D20" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D20" t="s">
-        <v>61</v>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D22" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C25" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
+        <v>73</v>
+      </c>
+      <c r="D26" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1368,8 +1459,9 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>